<commit_message>
add colored cmds in console and other. weather upd
</commit_message>
<xml_diff>
--- a/documents/todo-list.xlsx
+++ b/documents/todo-list.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>№</t>
   </si>
@@ -39,66 +39,72 @@
     <t>1.</t>
   </si>
   <si>
-    <t>Подкорректировать условия для добавления в список дел то есть если прилетает пустое условие то нужно выполнять другие действия</t>
-  </si>
-  <si>
     <t>Вывести отдельную команду для реакции на грубое поведение</t>
   </si>
   <si>
+    <t>расширить озвучивание списка дел</t>
+  </si>
+  <si>
     <t>2.</t>
   </si>
   <si>
-    <t>Почистить вентилятор</t>
-  </si>
-  <si>
     <t>Доработать фильтр плохих слов</t>
   </si>
   <si>
+    <t>почистить пылесос</t>
+  </si>
+  <si>
     <t>3.</t>
   </si>
   <si>
-    <t>Переписать функцию голосового поиска</t>
-  </si>
-  <si>
-    <t>Расширить список дел</t>
-  </si>
-  <si>
     <t>4.</t>
   </si>
   <si>
-    <t>Попробовать спарсить википедию</t>
-  </si>
-  <si>
-    <t>Модернизировать функционал погоды</t>
+    <t>Сделать реакцию на восторг</t>
   </si>
   <si>
     <t>5.</t>
   </si>
   <si>
-    <t>Сделать реакцию на восторг</t>
+    <t>Сделать более медленное cэмплирование</t>
   </si>
   <si>
     <t>6.</t>
   </si>
   <si>
-    <t>Сделать более медленное cэмплирование</t>
+    <t>модернизировать анекдоты</t>
   </si>
   <si>
     <t>7.</t>
   </si>
   <si>
+    <t>добавить возможность открывать ютуб</t>
+  </si>
+  <si>
     <t>8.</t>
   </si>
   <si>
+    <t>поискать переключение раскладки клавиатуры на питоне и расставлять знаки препинания в зависимости от раскладки</t>
+  </si>
+  <si>
     <t>9.</t>
   </si>
   <si>
+    <t>Добавить возможность поставить пробел</t>
+  </si>
+  <si>
     <t>10.</t>
   </si>
   <si>
+    <t>Улучшить фильтр для печати с клавиатуры</t>
+  </si>
+  <si>
     <t>11.</t>
   </si>
   <si>
+    <t>Добавить возможность сохранять файл</t>
+  </si>
+  <si>
     <t>12.</t>
   </si>
   <si>
@@ -150,7 +156,13 @@
     <t>28.</t>
   </si>
   <si>
-    <t>✔</t>
+    <t>29.</t>
+  </si>
+  <si>
+    <t>30.</t>
+  </si>
+  <si>
+    <t>31.</t>
   </si>
 </sst>
 </file>
@@ -234,7 +246,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -271,12 +283,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -406,7 +412,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -448,11 +454,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -733,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:D5"/>
+      <selection activeCell="B13" sqref="B13:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -782,26 +783,24 @@
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7"/>
       <c r="E3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="7"/>
-      <c r="H3" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="6"/>
@@ -818,14 +817,10 @@
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>12</v>
-      </c>
+      <c r="B5" s="5"/>
       <c r="C5" s="6"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="E5" s="5"/>
       <c r="F5" s="6"/>
       <c r="G5" s="7"/>
       <c r="H5" s="2"/>
@@ -833,16 +828,14 @@
     </row>
     <row r="6" spans="1:9" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="7"/>
-      <c r="E6" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="E6" s="5"/>
       <c r="F6" s="6"/>
       <c r="G6" s="7"/>
       <c r="H6" s="2"/>
@@ -850,10 +843,10 @@
     </row>
     <row r="7" spans="1:9" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="7"/>
@@ -865,10 +858,10 @@
     </row>
     <row r="8" spans="1:9" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="7"/>
@@ -880,9 +873,11 @@
     </row>
     <row r="9" spans="1:9" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="8"/>
+        <v>18</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>19</v>
+      </c>
       <c r="C9" s="6"/>
       <c r="D9" s="7"/>
       <c r="E9" s="5"/>
@@ -893,9 +888,11 @@
     </row>
     <row r="10" spans="1:9" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="8"/>
+        <v>20</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="C10" s="6"/>
       <c r="D10" s="7"/>
       <c r="E10" s="5"/>
@@ -906,9 +903,11 @@
     </row>
     <row r="11" spans="1:9" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="8"/>
       <c r="C11" s="6"/>
       <c r="D11" s="7"/>
       <c r="E11" s="5"/>
@@ -921,7 +920,9 @@
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="8"/>
+      <c r="B12" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="C12" s="6"/>
       <c r="D12" s="7"/>
       <c r="E12" s="5"/>
@@ -932,9 +933,11 @@
     </row>
     <row r="13" spans="1:9" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="8"/>
+        <v>26</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="C13" s="6"/>
       <c r="D13" s="7"/>
       <c r="E13" s="5"/>
@@ -945,7 +948,7 @@
     </row>
     <row r="14" spans="1:9" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="6"/>
@@ -958,7 +961,7 @@
     </row>
     <row r="15" spans="1:9" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="6"/>
@@ -971,7 +974,7 @@
     </row>
     <row r="16" spans="1:9" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="6"/>
@@ -984,7 +987,7 @@
     </row>
     <row r="17" spans="1:9" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="6"/>
@@ -997,7 +1000,7 @@
     </row>
     <row r="18" spans="1:9" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="6"/>
@@ -1010,7 +1013,7 @@
     </row>
     <row r="19" spans="1:9" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="6"/>
@@ -1023,7 +1026,7 @@
     </row>
     <row r="20" spans="1:9" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="6"/>
@@ -1036,7 +1039,7 @@
     </row>
     <row r="21" spans="1:9" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="6"/>
@@ -1049,7 +1052,7 @@
     </row>
     <row r="22" spans="1:9" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="6"/>
@@ -1062,7 +1065,7 @@
     </row>
     <row r="23" spans="1:9" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="6"/>
@@ -1075,7 +1078,7 @@
     </row>
     <row r="24" spans="1:9" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="6"/>
@@ -1088,7 +1091,7 @@
     </row>
     <row r="25" spans="1:9" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="6"/>
@@ -1101,7 +1104,7 @@
     </row>
     <row r="26" spans="1:9" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="6"/>
@@ -1114,7 +1117,7 @@
     </row>
     <row r="27" spans="1:9" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="6"/>
@@ -1127,7 +1130,7 @@
     </row>
     <row r="28" spans="1:9" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="6"/>
@@ -1140,7 +1143,7 @@
     </row>
     <row r="29" spans="1:9" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="6"/>
@@ -1153,7 +1156,7 @@
     </row>
     <row r="30" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="6"/>
@@ -1164,8 +1167,689 @@
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
     </row>
+    <row r="31" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="8"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+    </row>
+    <row r="32" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" s="8"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+    </row>
+    <row r="33" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="8"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+    </row>
+    <row r="34" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34" s="8"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+    </row>
+    <row r="35" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" s="8"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+    </row>
+    <row r="36" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" s="8"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+    </row>
+    <row r="37" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37" s="8"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+    </row>
+    <row r="38" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38" s="8"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+    </row>
+    <row r="39" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39" s="8"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+    </row>
+    <row r="40" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="B40" s="8"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+    </row>
+    <row r="41" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41" s="8"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+    </row>
+    <row r="42" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="B42" s="8"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+    </row>
+    <row r="43" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="B43" s="8"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+    </row>
+    <row r="44" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44" s="8"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+    </row>
+    <row r="45" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45" s="8"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+    </row>
+    <row r="46" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46" s="8"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+    </row>
+    <row r="47" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="B47" s="8"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+    </row>
+    <row r="48" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48" s="8"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+    </row>
+    <row r="49" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49" s="8"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
+    </row>
+    <row r="50" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50" s="8"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
+    </row>
+    <row r="51" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51" s="8"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
+    </row>
+    <row r="52" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52" s="8"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
+    </row>
+    <row r="53" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="1">
+        <v>51</v>
+      </c>
+      <c r="B53" s="8"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
+    </row>
+    <row r="54" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="1">
+        <v>52</v>
+      </c>
+      <c r="B54" s="8"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="3"/>
+      <c r="I54" s="3"/>
+    </row>
+    <row r="55" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="1">
+        <v>53</v>
+      </c>
+      <c r="B55" s="8"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="3"/>
+    </row>
+    <row r="56" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="1">
+        <v>54</v>
+      </c>
+      <c r="B56" s="8"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="7"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="3"/>
+    </row>
+    <row r="57" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="1">
+        <v>55</v>
+      </c>
+      <c r="B57" s="8"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="3"/>
+      <c r="I57" s="3"/>
+    </row>
+    <row r="58" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="1">
+        <v>56</v>
+      </c>
+      <c r="B58" s="8"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="7"/>
+      <c r="H58" s="3"/>
+      <c r="I58" s="3"/>
+    </row>
+    <row r="59" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="1">
+        <v>57</v>
+      </c>
+      <c r="B59" s="8"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="7"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="7"/>
+      <c r="H59" s="3"/>
+      <c r="I59" s="3"/>
+    </row>
+    <row r="60" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="1">
+        <v>58</v>
+      </c>
+      <c r="B60" s="8"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="7"/>
+      <c r="H60" s="3"/>
+      <c r="I60" s="3"/>
+    </row>
+    <row r="61" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="1">
+        <v>59</v>
+      </c>
+      <c r="B61" s="8"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="7"/>
+      <c r="H61" s="3"/>
+      <c r="I61" s="3"/>
+    </row>
+    <row r="62" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="1">
+        <v>60</v>
+      </c>
+      <c r="B62" s="8"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="7"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="3"/>
+      <c r="I62" s="3"/>
+    </row>
+    <row r="63" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="1">
+        <v>61</v>
+      </c>
+      <c r="B63" s="8"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="7"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="7"/>
+      <c r="H63" s="3"/>
+      <c r="I63" s="3"/>
+    </row>
+    <row r="64" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="1">
+        <v>62</v>
+      </c>
+      <c r="B64" s="8"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="7"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="7"/>
+      <c r="H64" s="3"/>
+      <c r="I64" s="3"/>
+    </row>
+    <row r="65" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="1">
+        <v>63</v>
+      </c>
+      <c r="B65" s="8"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="7"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="7"/>
+      <c r="H65" s="3"/>
+      <c r="I65" s="3"/>
+    </row>
+    <row r="66" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="1">
+        <v>64</v>
+      </c>
+      <c r="B66" s="8"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="7"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="7"/>
+      <c r="H66" s="3"/>
+      <c r="I66" s="3"/>
+    </row>
+    <row r="67" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="1">
+        <v>65</v>
+      </c>
+      <c r="B67" s="8"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="7"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="3"/>
+    </row>
+    <row r="68" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="1">
+        <v>66</v>
+      </c>
+      <c r="B68" s="8"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="7"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="7"/>
+      <c r="H68" s="3"/>
+      <c r="I68" s="3"/>
+    </row>
+    <row r="69" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="1">
+        <v>67</v>
+      </c>
+      <c r="B69" s="8"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="7"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="7"/>
+      <c r="H69" s="3"/>
+      <c r="I69" s="3"/>
+    </row>
+    <row r="70" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="1">
+        <v>68</v>
+      </c>
+      <c r="B70" s="8"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="7"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="7"/>
+      <c r="H70" s="3"/>
+      <c r="I70" s="3"/>
+    </row>
+    <row r="71" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="1">
+        <v>69</v>
+      </c>
+      <c r="B71" s="8"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="7"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="7"/>
+      <c r="H71" s="3"/>
+      <c r="I71" s="3"/>
+    </row>
+    <row r="72" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="1">
+        <v>70</v>
+      </c>
+      <c r="B72" s="8"/>
+      <c r="C72" s="6"/>
+      <c r="D72" s="7"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="7"/>
+      <c r="H72" s="3"/>
+      <c r="I72" s="3"/>
+    </row>
+    <row r="73" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="1">
+        <v>71</v>
+      </c>
+      <c r="B73" s="8"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="7"/>
+      <c r="E73" s="5"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="7"/>
+      <c r="H73" s="3"/>
+      <c r="I73" s="3"/>
+    </row>
+    <row r="74" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="1">
+        <v>72</v>
+      </c>
+      <c r="B74" s="8"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="7"/>
+      <c r="E74" s="5"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="7"/>
+      <c r="H74" s="3"/>
+      <c r="I74" s="3"/>
+    </row>
+    <row r="75" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="1">
+        <v>73</v>
+      </c>
+      <c r="B75" s="8"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="7"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="7"/>
+      <c r="H75" s="3"/>
+      <c r="I75" s="3"/>
+    </row>
+    <row r="76" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="1">
+        <v>74</v>
+      </c>
+      <c r="B76" s="8"/>
+      <c r="C76" s="6"/>
+      <c r="D76" s="7"/>
+      <c r="E76" s="5"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="7"/>
+      <c r="H76" s="3"/>
+      <c r="I76" s="3"/>
+    </row>
+    <row r="77" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="1">
+        <v>75</v>
+      </c>
+      <c r="B77" s="8"/>
+      <c r="C77" s="6"/>
+      <c r="D77" s="7"/>
+      <c r="E77" s="5"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="7"/>
+      <c r="H77" s="3"/>
+      <c r="I77" s="3"/>
+    </row>
+    <row r="78" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="1">
+        <v>76</v>
+      </c>
+      <c r="B78" s="8"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="5"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="7"/>
+      <c r="H78" s="3"/>
+      <c r="I78" s="3"/>
+    </row>
+    <row r="79" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="1">
+        <v>77</v>
+      </c>
+      <c r="B79" s="8"/>
+      <c r="C79" s="6"/>
+      <c r="D79" s="7"/>
+      <c r="E79" s="5"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="7"/>
+      <c r="H79" s="3"/>
+      <c r="I79" s="3"/>
+    </row>
+    <row r="80" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="1">
+        <v>78</v>
+      </c>
+      <c r="B80" s="8"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="7"/>
+      <c r="E80" s="5"/>
+      <c r="F80" s="6"/>
+      <c r="G80" s="7"/>
+      <c r="H80" s="3"/>
+      <c r="I80" s="3"/>
+    </row>
+    <row r="81" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="1">
+        <v>79</v>
+      </c>
+      <c r="B81" s="8"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="7"/>
+      <c r="E81" s="5"/>
+      <c r="F81" s="6"/>
+      <c r="G81" s="7"/>
+      <c r="H81" s="3"/>
+      <c r="I81" s="3"/>
+    </row>
+    <row r="82" spans="1:9" ht="18.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="1">
+        <v>80</v>
+      </c>
+      <c r="B82" s="8"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="7"/>
+      <c r="E82" s="5"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="7"/>
+      <c r="H82" s="3"/>
+      <c r="I82" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="61">
+  <mergeCells count="165">
+    <mergeCell ref="H1:I2"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
     <mergeCell ref="E29:G29"/>
     <mergeCell ref="E30:G30"/>
     <mergeCell ref="B29:D29"/>
@@ -1176,11 +1860,6 @@
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="B27:D27"/>
     <mergeCell ref="B28:D28"/>
-    <mergeCell ref="H1:I2"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E3:G3"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="E15:G15"/>
@@ -1190,6 +1869,11 @@
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="E25:G25"/>
     <mergeCell ref="E17:G17"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B34:D34"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B19:D19"/>
@@ -1197,20 +1881,13 @@
     <mergeCell ref="E22:G22"/>
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E13:G13"/>
     <mergeCell ref="E9:G9"/>
     <mergeCell ref="E8:G8"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="E12:G12"/>
+    <mergeCell ref="B35:D35"/>
     <mergeCell ref="E4:G4"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="A1:A2"/>
@@ -1227,6 +1904,112 @@
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="B79:D79"/>
+    <mergeCell ref="B80:D80"/>
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B70:D70"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B81:D81"/>
+    <mergeCell ref="B82:D82"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="B76:D76"/>
+    <mergeCell ref="B77:D77"/>
+    <mergeCell ref="B78:D78"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="E59:G59"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="E66:G66"/>
+    <mergeCell ref="E67:G67"/>
+    <mergeCell ref="E68:G68"/>
+    <mergeCell ref="E69:G69"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="E61:G61"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="E64:G64"/>
+    <mergeCell ref="E80:G80"/>
+    <mergeCell ref="E81:G81"/>
+    <mergeCell ref="E82:G82"/>
+    <mergeCell ref="E75:G75"/>
+    <mergeCell ref="E76:G76"/>
+    <mergeCell ref="E77:G77"/>
+    <mergeCell ref="E78:G78"/>
+    <mergeCell ref="E79:G79"/>
+    <mergeCell ref="E70:G70"/>
+    <mergeCell ref="E71:G71"/>
+    <mergeCell ref="E72:G72"/>
+    <mergeCell ref="E73:G73"/>
+    <mergeCell ref="E74:G74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>